<commit_message>
FEATURE: Get PIP TAGS
</commit_message>
<xml_diff>
--- a/files/PIB/optica-de-produção.xlsx
+++ b/files/PIB/optica-de-produção.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arlindo Boa\Desktop\tactic\files\PIB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71714CA3-1976-4A29-B0EB-8362E9E77454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD41768-C7F1-488C-BD48-FAB629C652AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,10 +16,18 @@
     <sheet name="Quadro.1" sheetId="1" r:id="rId1"/>
     <sheet name="Quadro.2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -936,14 +944,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ32"/>
+  <dimension ref="A1:AJ31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="M18" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D31" sqref="D31"/>
       <selection pane="topRight" activeCell="D31" sqref="D31"/>
       <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3016,599 +3024,566 @@
         <v>6723.9223022460938</v>
       </c>
     </row>
-    <row r="25" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="34"/>
-      <c r="B25" s="35"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="36"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="23"/>
-      <c r="M25" s="23"/>
-      <c r="N25" s="23"/>
-      <c r="O25" s="23"/>
-      <c r="P25" s="23"/>
-      <c r="Q25" s="23"/>
-      <c r="R25" s="23"/>
-      <c r="S25" s="23"/>
-      <c r="T25" s="23"/>
-      <c r="U25" s="23"/>
-      <c r="V25" s="23"/>
-      <c r="W25" s="23"/>
-      <c r="X25" s="23"/>
-      <c r="Y25" s="20"/>
-      <c r="Z25" s="23"/>
-      <c r="AA25" s="23"/>
-      <c r="AB25" s="23"/>
-      <c r="AC25" s="20"/>
-      <c r="AD25" s="20"/>
-      <c r="AE25" s="21"/>
+    <row r="25" spans="1:36" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="18">
+        <v>5121.5346626147466</v>
+      </c>
+      <c r="C25" s="19">
+        <v>6503.7982970539197</v>
+      </c>
+      <c r="D25" s="19">
+        <v>10341.972676708507</v>
+      </c>
+      <c r="E25" s="19">
+        <v>16600.878013198308</v>
+      </c>
+      <c r="F25" s="19">
+        <v>25676.072385345033</v>
+      </c>
+      <c r="G25" s="19">
+        <v>39814.863166492665</v>
+      </c>
+      <c r="H25" s="19">
+        <v>49595.416515169032</v>
+      </c>
+      <c r="I25" s="19">
+        <v>58089.783014492692</v>
+      </c>
+      <c r="J25" s="19">
+        <v>64259.693922695966</v>
+      </c>
+      <c r="K25" s="20">
+        <v>71432.691545370049</v>
+      </c>
+      <c r="L25" s="20">
+        <v>95930.226073689788</v>
+      </c>
+      <c r="M25" s="20">
+        <v>119966.81747967836</v>
+      </c>
+      <c r="N25" s="20">
+        <v>132462.94025718648</v>
+      </c>
+      <c r="O25" s="20">
+        <v>152423.82509593459</v>
+      </c>
+      <c r="P25" s="20">
+        <v>174847.85979899747</v>
+      </c>
+      <c r="Q25" s="20">
+        <v>208440.75320371211</v>
+      </c>
+      <c r="R25" s="20">
+        <v>243338.49743675822</v>
+      </c>
+      <c r="S25" s="20">
+        <v>275240.33641131734</v>
+      </c>
+      <c r="T25" s="20">
+        <v>296580.24767273496</v>
+      </c>
+      <c r="U25" s="20">
+        <v>340299.17639655445</v>
+      </c>
+      <c r="V25" s="20">
+        <v>374930.0767793656</v>
+      </c>
+      <c r="W25" s="20">
+        <v>415746.05112457275</v>
+      </c>
+      <c r="X25" s="20">
+        <v>452279.01923274994</v>
+      </c>
+      <c r="Y25" s="20">
+        <v>495547.06871795654</v>
+      </c>
+      <c r="Z25" s="20">
+        <v>564123.43133544922</v>
+      </c>
+      <c r="AA25" s="20">
+        <v>666945.25360488892</v>
+      </c>
+      <c r="AB25" s="20">
+        <v>756527.00646209717</v>
+      </c>
+      <c r="AC25" s="20">
+        <v>805235.11025619507</v>
+      </c>
+      <c r="AD25" s="20">
+        <v>855280.51029586792</v>
+      </c>
+      <c r="AE25" s="21">
+        <v>865763.03781975782</v>
+      </c>
     </row>
     <row r="26" spans="1:36" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B26" s="18">
-        <v>5121.5346626147466</v>
+        <v>90.586313187651001</v>
       </c>
       <c r="C26" s="19">
-        <v>6503.7982970539197</v>
+        <v>139.90795573158408</v>
       </c>
       <c r="D26" s="19">
-        <v>10341.972676708507</v>
+        <v>232.85220208068731</v>
       </c>
       <c r="E26" s="19">
-        <v>16600.878013198308</v>
+        <v>286.36871359895019</v>
       </c>
       <c r="F26" s="19">
-        <v>25676.072385345033</v>
+        <v>493.70128910082701</v>
       </c>
       <c r="G26" s="19">
-        <v>39814.863166492665</v>
+        <v>3742.6772130354584</v>
       </c>
       <c r="H26" s="19">
-        <v>49595.416515169032</v>
+        <v>4068.8426867845269</v>
       </c>
       <c r="I26" s="19">
-        <v>58089.783014492692</v>
+        <v>4416.6569868720271</v>
       </c>
       <c r="J26" s="19">
-        <v>64259.693922695966</v>
+        <v>12089.51651563319</v>
       </c>
       <c r="K26" s="20">
-        <v>71432.691545370049</v>
+        <v>14699.564083928453</v>
       </c>
       <c r="L26" s="20">
-        <v>95930.226073689788</v>
+        <v>15839.577640624684</v>
       </c>
       <c r="M26" s="20">
-        <v>119966.81747967836</v>
+        <v>14453.265269933363</v>
       </c>
       <c r="N26" s="20">
-        <v>132462.94025718648</v>
+        <v>17446.198937227615</v>
       </c>
       <c r="O26" s="20">
-        <v>152423.82509593459</v>
+        <v>19896.797046648629</v>
       </c>
       <c r="P26" s="20">
-        <v>174847.85979899747</v>
+        <v>22140.819048500605</v>
       </c>
       <c r="Q26" s="20">
-        <v>208440.75320371211</v>
+        <v>24659.570659101424</v>
       </c>
       <c r="R26" s="20">
-        <v>243338.49743675822</v>
+        <v>26714.428482452407</v>
       </c>
       <c r="S26" s="20">
-        <v>275240.33641131734</v>
+        <v>29882.740397275316</v>
       </c>
       <c r="T26" s="20">
-        <v>296580.24767273496</v>
+        <v>31285.7533344771</v>
       </c>
       <c r="U26" s="20">
-        <v>340299.17639655445</v>
+        <v>36815.802961852525</v>
       </c>
       <c r="V26" s="20">
-        <v>374930.0767793656</v>
+        <v>43107.13671875</v>
       </c>
       <c r="W26" s="20">
-        <v>415746.05112457275</v>
+        <v>48175.326171875</v>
       </c>
       <c r="X26" s="20">
-        <v>452279.01923274994</v>
+        <v>58717.6240234375</v>
       </c>
       <c r="Y26" s="20">
-        <v>495547.06871795654</v>
+        <v>59900.00146484375</v>
       </c>
       <c r="Z26" s="20">
-        <v>564123.43133544922</v>
+        <v>73636.1875</v>
       </c>
       <c r="AA26" s="20">
-        <v>666945.25360488892</v>
+        <v>85756.560546875</v>
       </c>
       <c r="AB26" s="20">
-        <v>756527.00646209717</v>
+        <v>83999.212890625</v>
       </c>
       <c r="AC26" s="20">
-        <v>805235.11025619507</v>
+        <v>90331.6083984375</v>
       </c>
       <c r="AD26" s="20">
-        <v>855280.51029586792</v>
+        <v>107340.28125</v>
       </c>
       <c r="AE26" s="21">
-        <v>865763.03781975782</v>
+        <v>108748.3232421875</v>
       </c>
     </row>
-    <row r="27" spans="1:36" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" s="18">
-        <v>90.586313187651001</v>
-      </c>
-      <c r="C27" s="19">
-        <v>139.90795573158408</v>
-      </c>
-      <c r="D27" s="19">
-        <v>232.85220208068731</v>
-      </c>
-      <c r="E27" s="19">
-        <v>286.36871359895019</v>
-      </c>
-      <c r="F27" s="19">
-        <v>493.70128910082701</v>
-      </c>
-      <c r="G27" s="19">
-        <v>3742.6772130354584</v>
-      </c>
-      <c r="H27" s="19">
-        <v>4068.8426867845269</v>
-      </c>
-      <c r="I27" s="19">
-        <v>4416.6569868720271</v>
-      </c>
-      <c r="J27" s="19">
-        <v>12089.51651563319</v>
-      </c>
-      <c r="K27" s="20">
-        <v>14699.564083928453</v>
-      </c>
-      <c r="L27" s="20">
-        <v>15839.577640624684</v>
-      </c>
-      <c r="M27" s="20">
-        <v>14453.265269933363</v>
-      </c>
-      <c r="N27" s="20">
-        <v>17446.198937227615</v>
-      </c>
-      <c r="O27" s="20">
-        <v>19896.797046648629</v>
-      </c>
-      <c r="P27" s="20">
-        <v>22140.819048500605</v>
-      </c>
-      <c r="Q27" s="20">
-        <v>24659.570659101424</v>
-      </c>
-      <c r="R27" s="20">
-        <v>26714.428482452407</v>
-      </c>
-      <c r="S27" s="20">
-        <v>29882.740397275316</v>
-      </c>
-      <c r="T27" s="20">
-        <v>31285.7533344771</v>
-      </c>
-      <c r="U27" s="20">
-        <v>36815.802961852525</v>
-      </c>
-      <c r="V27" s="20">
-        <v>43107.13671875</v>
-      </c>
-      <c r="W27" s="20">
-        <v>48175.326171875</v>
-      </c>
-      <c r="X27" s="20">
-        <v>58717.6240234375</v>
-      </c>
-      <c r="Y27" s="20">
-        <v>59900.00146484375</v>
-      </c>
-      <c r="Z27" s="20">
-        <v>73636.1875</v>
-      </c>
-      <c r="AA27" s="20">
-        <v>85756.560546875</v>
-      </c>
-      <c r="AB27" s="20">
-        <v>83999.212890625</v>
-      </c>
-      <c r="AC27" s="20">
-        <v>90331.6083984375</v>
-      </c>
-      <c r="AD27" s="20">
-        <v>107340.28125</v>
-      </c>
-      <c r="AE27" s="21">
-        <v>108748.3232421875</v>
+    <row r="27" spans="1:36" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="26"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="23">
+        <v>9584.0200954161555</v>
+      </c>
+      <c r="K27" s="23">
+        <v>11668.550511807836</v>
+      </c>
+      <c r="L27" s="23">
+        <v>12566.984560630424</v>
+      </c>
+      <c r="M27" s="23">
+        <v>11237.845944847966</v>
+      </c>
+      <c r="N27" s="23">
+        <v>13229.082669147945</v>
+      </c>
+      <c r="O27" s="23">
+        <v>14779.062769872069</v>
+      </c>
+      <c r="P27" s="23">
+        <v>16144.366424283424</v>
+      </c>
+      <c r="Q27" s="23">
+        <v>17921.391647062366</v>
+      </c>
+      <c r="R27" s="23">
+        <v>19365.30092778397</v>
+      </c>
+      <c r="S27" s="23">
+        <v>20145.449313459671</v>
+      </c>
+      <c r="T27" s="23">
+        <v>22068.5159564928</v>
+      </c>
+      <c r="U27" s="23">
+        <v>25859.137992772987</v>
+      </c>
+      <c r="V27" s="23">
+        <v>29519.4765625</v>
+      </c>
+      <c r="W27" s="23">
+        <v>32072.646484375</v>
+      </c>
+      <c r="X27" s="23">
+        <v>38703.4609375</v>
+      </c>
+      <c r="Y27" s="23">
+        <v>40131.703125</v>
+      </c>
+      <c r="Z27" s="23">
+        <v>51719.4453125</v>
+      </c>
+      <c r="AA27" s="23">
+        <v>59104.3671875</v>
+      </c>
+      <c r="AB27" s="23">
+        <v>58517.7734375</v>
+      </c>
+      <c r="AC27" s="23">
+        <v>65096.3515625</v>
+      </c>
+      <c r="AD27" s="23">
+        <v>73791.046875</v>
+      </c>
+      <c r="AE27" s="28">
+        <v>75498.34375</v>
       </c>
     </row>
     <row r="28" spans="1:36" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="27"/>
+        <v>65</v>
+      </c>
+      <c r="B28" s="38">
+        <v>90.586313187651001</v>
+      </c>
+      <c r="C28" s="23">
+        <v>139.90795573158408</v>
+      </c>
+      <c r="D28" s="23">
+        <v>232.85220208068731</v>
+      </c>
+      <c r="E28" s="23">
+        <v>286.36871359895019</v>
+      </c>
+      <c r="F28" s="23">
+        <v>493.70128910082701</v>
+      </c>
+      <c r="G28" s="23">
+        <v>575.55249351681164</v>
+      </c>
+      <c r="H28" s="23">
+        <v>682.58131496181659</v>
+      </c>
+      <c r="I28" s="23">
+        <v>804.49519343856684</v>
+      </c>
       <c r="J28" s="23">
-        <v>9584.0200954161555</v>
+        <v>847.5667563513374</v>
       </c>
       <c r="K28" s="23">
-        <v>11668.550511807836</v>
+        <v>1073.761512959489</v>
       </c>
       <c r="L28" s="23">
-        <v>12566.984560630424</v>
+        <v>1175.2018320598743</v>
       </c>
       <c r="M28" s="23">
-        <v>11237.845944847966</v>
+        <v>1555.7104775387893</v>
       </c>
       <c r="N28" s="23">
-        <v>13229.082669147945</v>
+        <v>1872.8571095047846</v>
       </c>
       <c r="O28" s="23">
-        <v>14779.062769872069</v>
+        <v>2058.5701857569993</v>
       </c>
       <c r="P28" s="23">
-        <v>16144.366424283424</v>
+        <v>2398.7451106095687</v>
       </c>
       <c r="Q28" s="23">
-        <v>17921.391647062366</v>
+        <v>2682.388671948152</v>
       </c>
       <c r="R28" s="23">
-        <v>19365.30092778397</v>
+        <v>3191.9515992785873</v>
       </c>
       <c r="S28" s="23">
-        <v>20145.449313459671</v>
+        <v>4733.3976770422441</v>
       </c>
       <c r="T28" s="23">
-        <v>22068.5159564928</v>
+        <v>4049.1800772244619</v>
       </c>
       <c r="U28" s="23">
-        <v>25859.137992772987</v>
+        <v>4437.2430029832803</v>
       </c>
       <c r="V28" s="23">
-        <v>29519.4765625</v>
+        <v>5834.59423828125</v>
       </c>
       <c r="W28" s="23">
-        <v>32072.646484375</v>
+        <v>8067.953125</v>
       </c>
       <c r="X28" s="23">
-        <v>38703.4609375</v>
+        <v>9004.099609375</v>
       </c>
       <c r="Y28" s="23">
-        <v>40131.703125</v>
+        <v>8124.31103515625</v>
       </c>
       <c r="Z28" s="23">
-        <v>51719.4453125</v>
+        <v>11036.1796875</v>
       </c>
       <c r="AA28" s="23">
-        <v>59104.3671875</v>
+        <v>12347.5859375</v>
       </c>
       <c r="AB28" s="23">
-        <v>58517.7734375</v>
+        <v>10726.4521484375</v>
       </c>
       <c r="AC28" s="23">
-        <v>65096.3515625</v>
+        <v>9846.97265625</v>
       </c>
       <c r="AD28" s="23">
-        <v>73791.046875</v>
+        <v>17154.529296875</v>
       </c>
       <c r="AE28" s="28">
-        <v>75498.34375</v>
+        <v>15103.4697265625</v>
       </c>
     </row>
-    <row r="29" spans="1:36" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="B29" s="38">
-        <v>90.586313187651001</v>
-      </c>
-      <c r="C29" s="23">
-        <v>139.90795573158408</v>
-      </c>
-      <c r="D29" s="23">
-        <v>232.85220208068731</v>
-      </c>
-      <c r="E29" s="23">
-        <v>286.36871359895019</v>
-      </c>
-      <c r="F29" s="23">
-        <v>493.70128910082701</v>
-      </c>
-      <c r="G29" s="23">
-        <v>575.55249351681164</v>
-      </c>
-      <c r="H29" s="23">
-        <v>682.58131496181659</v>
-      </c>
-      <c r="I29" s="23">
-        <v>804.49519343856684</v>
-      </c>
-      <c r="J29" s="23">
-        <v>847.5667563513374</v>
-      </c>
-      <c r="K29" s="23">
-        <v>1073.761512959489</v>
-      </c>
-      <c r="L29" s="23">
-        <v>1175.2018320598743</v>
-      </c>
-      <c r="M29" s="23">
-        <v>1555.7104775387893</v>
-      </c>
-      <c r="N29" s="23">
-        <v>1872.8571095047846</v>
-      </c>
-      <c r="O29" s="23">
-        <v>2058.5701857569993</v>
-      </c>
-      <c r="P29" s="23">
-        <v>2398.7451106095687</v>
-      </c>
-      <c r="Q29" s="23">
-        <v>2682.388671948152</v>
-      </c>
-      <c r="R29" s="23">
-        <v>3191.9515992785873</v>
-      </c>
-      <c r="S29" s="23">
-        <v>4733.3976770422441</v>
-      </c>
-      <c r="T29" s="23">
-        <v>4049.1800772244619</v>
-      </c>
-      <c r="U29" s="23">
-        <v>4437.2430029832803</v>
-      </c>
-      <c r="V29" s="23">
-        <v>5834.59423828125</v>
-      </c>
-      <c r="W29" s="23">
-        <v>8067.953125</v>
-      </c>
-      <c r="X29" s="23">
-        <v>9004.099609375</v>
-      </c>
-      <c r="Y29" s="23">
-        <v>8124.31103515625</v>
-      </c>
-      <c r="Z29" s="23">
-        <v>11036.1796875</v>
-      </c>
-      <c r="AA29" s="23">
-        <v>12347.5859375</v>
-      </c>
-      <c r="AB29" s="23">
-        <v>10726.4521484375</v>
-      </c>
-      <c r="AC29" s="23">
-        <v>9846.97265625</v>
-      </c>
-      <c r="AD29" s="23">
-        <v>17154.529296875</v>
-      </c>
-      <c r="AE29" s="28">
-        <v>15103.4697265625</v>
+    <row r="29" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="40"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="42">
+        <v>3167.1247195186465</v>
+      </c>
+      <c r="H29" s="42">
+        <v>3386.2613718227103</v>
+      </c>
+      <c r="I29" s="42">
+        <v>3612.1617934334599</v>
+      </c>
+      <c r="J29" s="42">
+        <v>1657.9296638656954</v>
+      </c>
+      <c r="K29" s="42">
+        <v>1957.2520591611274</v>
+      </c>
+      <c r="L29" s="42">
+        <v>2097.3912479343844</v>
+      </c>
+      <c r="M29" s="42">
+        <v>1659.708847546608</v>
+      </c>
+      <c r="N29" s="42">
+        <v>2344.2591585748842</v>
+      </c>
+      <c r="O29" s="42">
+        <v>3059.1640910195588</v>
+      </c>
+      <c r="P29" s="42">
+        <v>3597.7075136076141</v>
+      </c>
+      <c r="Q29" s="42">
+        <v>4055.7903400909072</v>
+      </c>
+      <c r="R29" s="42">
+        <v>4157.1759553898519</v>
+      </c>
+      <c r="S29" s="42">
+        <v>5003.8934067734008</v>
+      </c>
+      <c r="T29" s="42">
+        <v>5168.0573007598377</v>
+      </c>
+      <c r="U29" s="42">
+        <v>6519.421966096259</v>
+      </c>
+      <c r="V29" s="42">
+        <v>7753.06591796875</v>
+      </c>
+      <c r="W29" s="42">
+        <v>8034.7265625</v>
+      </c>
+      <c r="X29" s="42">
+        <v>11010.0634765625</v>
+      </c>
+      <c r="Y29" s="42">
+        <v>11643.9873046875</v>
+      </c>
+      <c r="Z29" s="42">
+        <v>10880.5625</v>
+      </c>
+      <c r="AA29" s="42">
+        <v>14304.607421875</v>
+      </c>
+      <c r="AB29" s="42">
+        <v>14754.9873046875</v>
+      </c>
+      <c r="AC29" s="42">
+        <v>15388.2841796875</v>
+      </c>
+      <c r="AD29" s="42">
+        <v>16394.705078125</v>
+      </c>
+      <c r="AE29" s="43">
+        <v>18146.509765625</v>
       </c>
     </row>
-    <row r="30" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="42">
-        <v>3167.1247195186465</v>
-      </c>
-      <c r="H30" s="42">
-        <v>3386.2613718227103</v>
-      </c>
-      <c r="I30" s="42">
-        <v>3612.1617934334599</v>
-      </c>
-      <c r="J30" s="42">
-        <v>1657.9296638656954</v>
-      </c>
-      <c r="K30" s="42">
-        <v>1957.2520591611274</v>
-      </c>
-      <c r="L30" s="42">
-        <v>2097.3912479343844</v>
-      </c>
-      <c r="M30" s="42">
-        <v>1659.708847546608</v>
-      </c>
-      <c r="N30" s="42">
-        <v>2344.2591585748842</v>
-      </c>
-      <c r="O30" s="42">
-        <v>3059.1640910195588</v>
-      </c>
-      <c r="P30" s="42">
-        <v>3597.7075136076141</v>
-      </c>
-      <c r="Q30" s="42">
-        <v>4055.7903400909072</v>
-      </c>
-      <c r="R30" s="42">
-        <v>4157.1759553898519</v>
-      </c>
-      <c r="S30" s="42">
-        <v>5003.8934067734008</v>
-      </c>
-      <c r="T30" s="42">
-        <v>5168.0573007598377</v>
-      </c>
-      <c r="U30" s="42">
-        <v>6519.421966096259</v>
-      </c>
-      <c r="V30" s="42">
-        <v>7753.06591796875</v>
-      </c>
-      <c r="W30" s="42">
-        <v>8034.7265625</v>
-      </c>
-      <c r="X30" s="42">
-        <v>11010.0634765625</v>
-      </c>
-      <c r="Y30" s="42">
-        <v>11643.9873046875</v>
-      </c>
-      <c r="Z30" s="42">
-        <v>10880.5625</v>
-      </c>
-      <c r="AA30" s="42">
-        <v>14304.607421875</v>
-      </c>
-      <c r="AB30" s="42">
-        <v>14754.9873046875</v>
-      </c>
-      <c r="AC30" s="42">
-        <v>15388.2841796875</v>
-      </c>
-      <c r="AD30" s="42">
-        <v>16394.705078125</v>
-      </c>
-      <c r="AE30" s="43">
-        <v>18146.509765625</v>
-      </c>
+    <row r="30" spans="1:36" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="46">
+        <v>5212.1209758023961</v>
+      </c>
+      <c r="C30" s="47">
+        <v>6643.7062527855051</v>
+      </c>
+      <c r="D30" s="47">
+        <v>10574.824878789193</v>
+      </c>
+      <c r="E30" s="47">
+        <v>16887.246726797253</v>
+      </c>
+      <c r="F30" s="47">
+        <v>26169.773674445856</v>
+      </c>
+      <c r="G30" s="47">
+        <v>43557.540379528131</v>
+      </c>
+      <c r="H30" s="47">
+        <v>53664.259201953559</v>
+      </c>
+      <c r="I30" s="47">
+        <v>62506.440001364725</v>
+      </c>
+      <c r="J30" s="47">
+        <v>76349.210438329159</v>
+      </c>
+      <c r="K30" s="48">
+        <v>86132.255629298481</v>
+      </c>
+      <c r="L30" s="48">
+        <v>111769.8037143145</v>
+      </c>
+      <c r="M30" s="48">
+        <v>134420.0827496117</v>
+      </c>
+      <c r="N30" s="48">
+        <v>149909.13919441408</v>
+      </c>
+      <c r="O30" s="48">
+        <v>172320.62214258322</v>
+      </c>
+      <c r="P30" s="48">
+        <v>196988.67884749809</v>
+      </c>
+      <c r="Q30" s="48">
+        <v>233100.32386281359</v>
+      </c>
+      <c r="R30" s="48">
+        <v>270052.92591921065</v>
+      </c>
+      <c r="S30" s="48">
+        <v>305123.07680859265</v>
+      </c>
+      <c r="T30" s="48">
+        <v>327866.00100721203</v>
+      </c>
+      <c r="U30" s="48">
+        <v>377114.97935840697</v>
+      </c>
+      <c r="V30" s="48">
+        <v>418037.21349811554</v>
+      </c>
+      <c r="W30" s="48">
+        <v>463921.37729644781</v>
+      </c>
+      <c r="X30" s="48">
+        <v>510996.64325618738</v>
+      </c>
+      <c r="Y30" s="48">
+        <v>555447.07018280029</v>
+      </c>
+      <c r="Z30" s="48">
+        <v>637759.61883544922</v>
+      </c>
+      <c r="AA30" s="48">
+        <v>752701.81415176392</v>
+      </c>
+      <c r="AB30" s="48">
+        <v>840526.21935272205</v>
+      </c>
+      <c r="AC30" s="48">
+        <v>895566.71865463268</v>
+      </c>
+      <c r="AD30" s="48">
+        <v>962620.79154586792</v>
+      </c>
+      <c r="AE30" s="49">
+        <v>974511.36106194521</v>
+      </c>
+      <c r="AF30" s="50"/>
+      <c r="AG30" s="50"/>
+      <c r="AH30" s="50"/>
+      <c r="AI30" s="50"/>
+      <c r="AJ30" s="50"/>
     </row>
-    <row r="31" spans="1:36" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B31" s="46">
-        <v>5212.1209758023961</v>
-      </c>
-      <c r="C31" s="47">
-        <v>6643.7062527855051</v>
-      </c>
-      <c r="D31" s="47">
-        <v>10574.824878789193</v>
-      </c>
-      <c r="E31" s="47">
-        <v>16887.246726797253</v>
-      </c>
-      <c r="F31" s="47">
-        <v>26169.773674445856</v>
-      </c>
-      <c r="G31" s="47">
-        <v>43557.540379528131</v>
-      </c>
-      <c r="H31" s="47">
-        <v>53664.259201953559</v>
-      </c>
-      <c r="I31" s="47">
-        <v>62506.440001364725</v>
-      </c>
-      <c r="J31" s="47">
-        <v>76349.210438329159</v>
-      </c>
-      <c r="K31" s="48">
-        <v>86132.255629298481</v>
-      </c>
-      <c r="L31" s="48">
-        <v>111769.8037143145</v>
-      </c>
-      <c r="M31" s="48">
-        <v>134420.0827496117</v>
-      </c>
-      <c r="N31" s="48">
-        <v>149909.13919441408</v>
-      </c>
-      <c r="O31" s="48">
-        <v>172320.62214258322</v>
-      </c>
-      <c r="P31" s="48">
-        <v>196988.67884749809</v>
-      </c>
-      <c r="Q31" s="48">
-        <v>233100.32386281359</v>
-      </c>
-      <c r="R31" s="48">
-        <v>270052.92591921065</v>
-      </c>
-      <c r="S31" s="48">
-        <v>305123.07680859265</v>
-      </c>
-      <c r="T31" s="48">
-        <v>327866.00100721203</v>
-      </c>
-      <c r="U31" s="48">
-        <v>377114.97935840697</v>
-      </c>
-      <c r="V31" s="48">
-        <v>418037.21349811554</v>
-      </c>
-      <c r="W31" s="48">
-        <v>463921.37729644781</v>
-      </c>
-      <c r="X31" s="48">
-        <v>510996.64325618738</v>
-      </c>
-      <c r="Y31" s="48">
-        <v>555447.07018280029</v>
-      </c>
-      <c r="Z31" s="48">
-        <v>637759.61883544922</v>
-      </c>
-      <c r="AA31" s="48">
-        <v>752701.81415176392</v>
-      </c>
-      <c r="AB31" s="48">
-        <v>840526.21935272205</v>
-      </c>
-      <c r="AC31" s="48">
-        <v>895566.71865463268</v>
-      </c>
-      <c r="AD31" s="48">
-        <v>962620.79154586792</v>
-      </c>
-      <c r="AE31" s="49">
-        <v>974511.36106194521</v>
-      </c>
-      <c r="AF31" s="50"/>
-      <c r="AG31" s="50"/>
-      <c r="AH31" s="50"/>
-      <c r="AI31" s="50"/>
-      <c r="AJ31" s="50"/>
-    </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A32" s="51"/>
-      <c r="B32" s="51"/>
-      <c r="C32" s="51"/>
-      <c r="D32" s="51"/>
-      <c r="E32" s="51"/>
-      <c r="F32" s="51"/>
-      <c r="G32" s="51"/>
-      <c r="H32" s="51"/>
-      <c r="I32" s="51"/>
-      <c r="J32" s="51"/>
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A31" s="51"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="51"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>